<commit_message>
06.08.19 Today sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
+++ b/August/Others/Requisition of Tulip-2/Requisition of Tulip-2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
   <si>
     <t>Model Name</t>
   </si>
@@ -373,10 +373,16 @@
     <t>Dark_Blue</t>
   </si>
   <si>
-    <t>05.08.19</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Gold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold </t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>07.08.19</t>
   </si>
 </sst>
 </file>
@@ -574,7 +580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -666,6 +672,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -699,6 +708,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -997,13 +1009,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:BC95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F87" sqref="F87"/>
+      <selection pane="bottomRight" activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1017,26 +1029,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="12.75">
-      <c r="A1" s="35"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5" s="6" customFormat="1" ht="15.75">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41"/>
     </row>
     <row r="3" spans="1:5" s="6" customFormat="1" ht="15">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="45"/>
+      <c r="B3" s="46"/>
       <c r="C3" s="20" t="s">
         <v>65</v>
       </c>
@@ -1044,7 +1056,7 @@
         <v>27</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" ht="12.75">
@@ -1172,19 +1184,17 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="5" customFormat="1" ht="15">
+    <row r="12" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
       <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="9">
         <v>896.23500000000001</v>
       </c>
-      <c r="C12" s="8">
-        <v>80</v>
-      </c>
+      <c r="C12" s="8"/>
       <c r="D12" s="12">
         <f t="shared" si="0"/>
-        <v>71698.8</v>
+        <v>0</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>85</v>
@@ -1245,7 +1255,7 @@
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="10">
-        <f>B16*C16</f>
+        <f>C16*B16</f>
         <v>0</v>
       </c>
       <c r="E16" s="8" t="s">
@@ -1332,22 +1342,20 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15">
+    <row r="22" spans="1:5" ht="15" hidden="1">
       <c r="A22" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="9">
         <v>1140.845</v>
       </c>
-      <c r="C22" s="8">
-        <v>40</v>
-      </c>
+      <c r="C22" s="8"/>
       <c r="D22" s="12">
         <f>C22*B22</f>
-        <v>45633.8</v>
+        <v>0</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="5" customFormat="1" ht="15" hidden="1">
@@ -1380,19 +1388,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15">
+    <row r="25" spans="1:5" ht="15" hidden="1">
       <c r="A25" s="8" t="s">
         <v>93</v>
       </c>
       <c r="B25" s="9">
         <v>907.26</v>
       </c>
-      <c r="C25" s="8">
-        <v>40</v>
-      </c>
+      <c r="C25" s="8"/>
       <c r="D25" s="10">
         <f t="shared" si="0"/>
-        <v>36290.400000000001</v>
+        <v>0</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>85</v>
@@ -1504,19 +1510,23 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:5" ht="15" hidden="1">
+    <row r="33" spans="1:5" ht="15">
       <c r="A33" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="9">
         <v>5607.9849999999997</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="8">
+        <v>7</v>
+      </c>
       <c r="D33" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="8"/>
+        <v>39255.894999999997</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="15" hidden="1">
       <c r="A34" s="8" t="s">
@@ -1562,17 +1572,19 @@
       </c>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="15" hidden="1">
+    <row r="37" spans="1:5" ht="15">
       <c r="A37" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="9">
         <v>6369.8850000000002</v>
       </c>
-      <c r="C37" s="8"/>
+      <c r="C37" s="8">
+        <v>7</v>
+      </c>
       <c r="D37" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44589.195</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>84</v>
@@ -1867,11 +1879,11 @@
         <v>5607.9849999999997</v>
       </c>
       <c r="C57" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D57" s="10">
         <f t="shared" si="0"/>
-        <v>28039.924999999999</v>
+        <v>39255.894999999997</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>84</v>
@@ -1935,19 +1947,17 @@
       </c>
       <c r="E61" s="8"/>
     </row>
-    <row r="62" spans="1:5" ht="15">
+    <row r="62" spans="1:5" ht="15" hidden="1">
       <c r="A62" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B62" s="9">
         <v>4896.21</v>
       </c>
-      <c r="C62" s="8">
-        <v>5</v>
-      </c>
+      <c r="C62" s="8"/>
       <c r="D62" s="10">
         <f t="shared" si="1"/>
-        <v>24481.05</v>
+        <v>0</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>84</v>
@@ -1980,28 +1990,76 @@
         <v>0</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:55" ht="15" hidden="1">
       <c r="A65" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B65" s="9">
         <v>4701.7299999999996</v>
       </c>
-      <c r="C65" s="8">
-        <v>5</v>
-      </c>
+      <c r="C65" s="8"/>
       <c r="D65" s="10">
         <f t="shared" si="1"/>
-        <v>23508.649999999998</v>
+        <v>0</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="15" hidden="1">
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
+      <c r="K65" s="47"/>
+      <c r="L65" s="47"/>
+      <c r="M65" s="47"/>
+      <c r="N65" s="47"/>
+      <c r="O65" s="47"/>
+      <c r="P65" s="47"/>
+      <c r="Q65" s="47"/>
+      <c r="R65" s="47"/>
+      <c r="S65" s="47"/>
+      <c r="T65" s="47"/>
+      <c r="U65" s="47"/>
+      <c r="V65" s="47"/>
+      <c r="W65" s="47"/>
+      <c r="X65" s="47"/>
+      <c r="Y65" s="47"/>
+      <c r="Z65" s="47"/>
+      <c r="AA65" s="47"/>
+      <c r="AB65" s="47"/>
+      <c r="AC65" s="47"/>
+      <c r="AD65" s="47"/>
+      <c r="AE65" s="47"/>
+      <c r="AF65" s="47"/>
+      <c r="AG65" s="47"/>
+      <c r="AH65" s="47"/>
+      <c r="AI65" s="47"/>
+      <c r="AJ65" s="47"/>
+      <c r="AK65" s="47"/>
+      <c r="AL65" s="47"/>
+      <c r="AM65" s="47"/>
+      <c r="AN65" s="47"/>
+      <c r="AO65" s="47"/>
+      <c r="AP65" s="47"/>
+      <c r="AQ65" s="47"/>
+      <c r="AR65" s="47"/>
+      <c r="AS65" s="47"/>
+      <c r="AT65" s="47"/>
+      <c r="AU65" s="47"/>
+      <c r="AV65" s="47"/>
+      <c r="AW65" s="47"/>
+      <c r="AX65" s="47"/>
+      <c r="AY65" s="47"/>
+      <c r="AZ65" s="47"/>
+      <c r="BA65" s="47"/>
+      <c r="BB65" s="47"/>
+      <c r="BC65" s="47"/>
+    </row>
+    <row r="66" spans="1:55" ht="15" hidden="1">
       <c r="A66" s="8" t="s">
         <v>50</v>
       </c>
@@ -2015,7 +2073,7 @@
       </c>
       <c r="E66" s="8"/>
     </row>
-    <row r="67" spans="1:5" ht="15" hidden="1">
+    <row r="67" spans="1:55" ht="15" hidden="1">
       <c r="A67" s="8" t="s">
         <v>55</v>
       </c>
@@ -2027,9 +2085,11 @@
         <f>C67*B67</f>
         <v>0</v>
       </c>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" spans="1:5" ht="15" hidden="1">
+      <c r="E67" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:55" ht="15" hidden="1">
       <c r="A68" s="8" t="s">
         <v>10</v>
       </c>
@@ -2043,7 +2103,7 @@
       </c>
       <c r="E68" s="8"/>
     </row>
-    <row r="69" spans="1:5" ht="15" hidden="1">
+    <row r="69" spans="1:55" ht="15" hidden="1">
       <c r="A69" s="8" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2119,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" hidden="1">
+    <row r="70" spans="1:55" ht="15" hidden="1">
       <c r="A70" s="8" t="s">
         <v>78</v>
       </c>
@@ -2075,7 +2135,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15" hidden="1">
+    <row r="71" spans="1:55" ht="15" hidden="1">
       <c r="A71" s="8" t="s">
         <v>56</v>
       </c>
@@ -2091,7 +2151,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15" hidden="1">
+    <row r="72" spans="1:55" ht="15" hidden="1">
       <c r="A72" s="8" t="s">
         <v>39</v>
       </c>
@@ -2107,7 +2167,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15" hidden="1">
+    <row r="73" spans="1:55" ht="15" hidden="1">
       <c r="A73" s="8" t="s">
         <v>73</v>
       </c>
@@ -2123,7 +2183,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15" hidden="1">
+    <row r="74" spans="1:55" ht="15" hidden="1">
       <c r="A74" s="8" t="s">
         <v>11</v>
       </c>
@@ -2137,7 +2197,7 @@
       </c>
       <c r="E74" s="8"/>
     </row>
-    <row r="75" spans="1:5" ht="15" hidden="1">
+    <row r="75" spans="1:55" ht="15" hidden="1">
       <c r="A75" s="8" t="s">
         <v>40</v>
       </c>
@@ -2151,7 +2211,7 @@
       </c>
       <c r="E75" s="8"/>
     </row>
-    <row r="76" spans="1:5" ht="15" hidden="1">
+    <row r="76" spans="1:55" ht="15" hidden="1">
       <c r="A76" s="8" t="s">
         <v>61</v>
       </c>
@@ -2167,7 +2227,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15" hidden="1">
+    <row r="77" spans="1:55" ht="15" hidden="1">
       <c r="A77" s="8" t="s">
         <v>72</v>
       </c>
@@ -2183,7 +2243,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="14.25" hidden="1" customHeight="1">
+    <row r="78" spans="1:55" ht="14.25" hidden="1" customHeight="1">
       <c r="A78" s="8" t="s">
         <v>89</v>
       </c>
@@ -2199,7 +2259,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="14.25" hidden="1" customHeight="1">
+    <row r="79" spans="1:55" ht="14.25" hidden="1" customHeight="1">
       <c r="A79" s="8" t="s">
         <v>98</v>
       </c>
@@ -2214,8 +2274,58 @@
       <c r="E79" s="8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" ht="15" hidden="1">
+      <c r="F79" s="47"/>
+      <c r="G79" s="47"/>
+      <c r="H79" s="47"/>
+      <c r="I79" s="47"/>
+      <c r="J79" s="47"/>
+      <c r="K79" s="47"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="47"/>
+      <c r="O79" s="47"/>
+      <c r="P79" s="47"/>
+      <c r="Q79" s="47"/>
+      <c r="R79" s="47"/>
+      <c r="S79" s="47"/>
+      <c r="T79" s="47"/>
+      <c r="U79" s="47"/>
+      <c r="V79" s="47"/>
+      <c r="W79" s="47"/>
+      <c r="X79" s="47"/>
+      <c r="Y79" s="47"/>
+      <c r="Z79" s="47"/>
+      <c r="AA79" s="47"/>
+      <c r="AB79" s="47"/>
+      <c r="AC79" s="47"/>
+      <c r="AD79" s="47"/>
+      <c r="AE79" s="47"/>
+      <c r="AF79" s="47"/>
+      <c r="AG79" s="47"/>
+      <c r="AH79" s="47"/>
+      <c r="AI79" s="47"/>
+      <c r="AJ79" s="47"/>
+      <c r="AK79" s="47"/>
+      <c r="AL79" s="47"/>
+      <c r="AM79" s="47"/>
+      <c r="AN79" s="47"/>
+      <c r="AO79" s="47"/>
+      <c r="AP79" s="47"/>
+      <c r="AQ79" s="47"/>
+      <c r="AR79" s="47"/>
+      <c r="AS79" s="47"/>
+      <c r="AT79" s="47"/>
+      <c r="AU79" s="47"/>
+      <c r="AV79" s="47"/>
+      <c r="AW79" s="47"/>
+      <c r="AX79" s="47"/>
+      <c r="AY79" s="47"/>
+      <c r="AZ79" s="47"/>
+      <c r="BA79" s="47"/>
+      <c r="BB79" s="47"/>
+      <c r="BC79" s="47"/>
+    </row>
+    <row r="80" spans="1:55" ht="15" hidden="1">
       <c r="A80" s="8" t="s">
         <v>71</v>
       </c>
@@ -2229,50 +2339,200 @@
       </c>
       <c r="E80" s="8"/>
     </row>
-    <row r="81" spans="1:9" s="2" customFormat="1" ht="15">
-      <c r="A81" s="41" t="s">
+    <row r="81" spans="1:55" s="2" customFormat="1" ht="15">
+      <c r="A81" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B81" s="41"/>
+      <c r="B81" s="42"/>
       <c r="C81" s="18">
         <f>SUM(C5:C80)</f>
-        <v>215</v>
+        <v>61</v>
       </c>
       <c r="D81" s="19">
         <f>SUM(D5:D80)</f>
-        <v>263978.22499999998</v>
-      </c>
-      <c r="E81" s="18"/>
-    </row>
-    <row r="82" spans="1:9" ht="17.25" customHeight="1">
+        <v>157426.58499999999</v>
+      </c>
+      <c r="E81" s="35"/>
+      <c r="F81" s="48"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="48"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="48"/>
+      <c r="K81" s="48"/>
+      <c r="L81" s="48"/>
+      <c r="M81" s="48"/>
+      <c r="N81" s="48"/>
+      <c r="O81" s="48"/>
+      <c r="P81" s="48"/>
+      <c r="Q81" s="48"/>
+      <c r="R81" s="48"/>
+      <c r="S81" s="48"/>
+      <c r="T81" s="48"/>
+      <c r="U81" s="48"/>
+      <c r="V81" s="48"/>
+      <c r="W81" s="48"/>
+      <c r="X81" s="48"/>
+      <c r="Y81" s="48"/>
+      <c r="Z81" s="48"/>
+      <c r="AA81" s="48"/>
+      <c r="AB81" s="48"/>
+      <c r="AC81" s="48"/>
+      <c r="AD81" s="48"/>
+      <c r="AE81" s="48"/>
+      <c r="AF81" s="48"/>
+      <c r="AG81" s="48"/>
+      <c r="AH81" s="48"/>
+      <c r="AI81" s="48"/>
+      <c r="AJ81" s="48"/>
+      <c r="AK81" s="48"/>
+      <c r="AL81" s="48"/>
+      <c r="AM81" s="48"/>
+      <c r="AN81" s="48"/>
+      <c r="AO81" s="48"/>
+      <c r="AP81" s="48"/>
+      <c r="AQ81" s="48"/>
+      <c r="AR81" s="48"/>
+      <c r="AS81" s="48"/>
+      <c r="AT81" s="48"/>
+      <c r="AU81" s="48"/>
+      <c r="AV81" s="48"/>
+      <c r="AW81" s="48"/>
+      <c r="AX81" s="48"/>
+      <c r="AY81" s="48"/>
+      <c r="AZ81" s="48"/>
+      <c r="BA81" s="48"/>
+      <c r="BB81" s="48"/>
+      <c r="BC81" s="48"/>
+    </row>
+    <row r="82" spans="1:55" ht="17.25" customHeight="1">
       <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A83" s="43"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="43"/>
-      <c r="D83" s="43"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="47"/>
+      <c r="H82" s="47"/>
+      <c r="I82" s="47"/>
+      <c r="J82" s="47"/>
+      <c r="K82" s="47"/>
+      <c r="L82" s="47"/>
+      <c r="M82" s="47"/>
+      <c r="N82" s="47"/>
+      <c r="O82" s="47"/>
+      <c r="P82" s="47"/>
+      <c r="Q82" s="47"/>
+      <c r="R82" s="47"/>
+      <c r="S82" s="47"/>
+      <c r="T82" s="47"/>
+      <c r="U82" s="47"/>
+      <c r="V82" s="47"/>
+      <c r="W82" s="47"/>
+      <c r="X82" s="47"/>
+      <c r="Y82" s="47"/>
+      <c r="Z82" s="47"/>
+      <c r="AA82" s="47"/>
+      <c r="AB82" s="47"/>
+      <c r="AC82" s="47"/>
+      <c r="AD82" s="47"/>
+      <c r="AE82" s="47"/>
+      <c r="AF82" s="47"/>
+      <c r="AG82" s="47"/>
+      <c r="AH82" s="47"/>
+      <c r="AI82" s="47"/>
+      <c r="AJ82" s="47"/>
+      <c r="AK82" s="47"/>
+      <c r="AL82" s="47"/>
+      <c r="AM82" s="47"/>
+      <c r="AN82" s="47"/>
+      <c r="AO82" s="47"/>
+      <c r="AP82" s="47"/>
+      <c r="AQ82" s="47"/>
+      <c r="AR82" s="47"/>
+      <c r="AS82" s="47"/>
+      <c r="AT82" s="47"/>
+      <c r="AU82" s="47"/>
+      <c r="AV82" s="47"/>
+      <c r="AW82" s="47"/>
+      <c r="AX82" s="47"/>
+      <c r="AY82" s="47"/>
+      <c r="AZ82" s="47"/>
+      <c r="BA82" s="47"/>
+      <c r="BB82" s="47"/>
+      <c r="BC82" s="47"/>
+    </row>
+    <row r="83" spans="1:55" s="16" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A83" s="44"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
       <c r="E83" s="25"/>
-    </row>
-    <row r="84" spans="1:9" s="16" customFormat="1" ht="17.25" customHeight="1">
+      <c r="F83" s="49"/>
+      <c r="G83" s="49"/>
+      <c r="H83" s="49"/>
+      <c r="I83" s="49"/>
+      <c r="J83" s="49"/>
+      <c r="K83" s="49"/>
+      <c r="L83" s="49"/>
+      <c r="M83" s="49"/>
+      <c r="N83" s="49"/>
+      <c r="O83" s="49"/>
+      <c r="P83" s="49"/>
+      <c r="Q83" s="49"/>
+      <c r="R83" s="49"/>
+      <c r="S83" s="49"/>
+      <c r="T83" s="49"/>
+      <c r="U83" s="49"/>
+      <c r="V83" s="49"/>
+      <c r="W83" s="49"/>
+      <c r="X83" s="49"/>
+      <c r="Y83" s="49"/>
+      <c r="Z83" s="49"/>
+      <c r="AA83" s="49"/>
+      <c r="AB83" s="49"/>
+      <c r="AC83" s="49"/>
+      <c r="AD83" s="49"/>
+      <c r="AE83" s="49"/>
+      <c r="AF83" s="49"/>
+      <c r="AG83" s="49"/>
+      <c r="AH83" s="49"/>
+      <c r="AI83" s="49"/>
+      <c r="AJ83" s="49"/>
+      <c r="AK83" s="49"/>
+      <c r="AL83" s="49"/>
+      <c r="AM83" s="49"/>
+      <c r="AN83" s="49"/>
+      <c r="AO83" s="49"/>
+      <c r="AP83" s="49"/>
+      <c r="AQ83" s="49"/>
+      <c r="AR83" s="49"/>
+      <c r="AS83" s="49"/>
+      <c r="AT83" s="49"/>
+      <c r="AU83" s="49"/>
+      <c r="AV83" s="49"/>
+      <c r="AW83" s="49"/>
+      <c r="AX83" s="49"/>
+      <c r="AY83" s="49"/>
+      <c r="AZ83" s="49"/>
+      <c r="BA83" s="49"/>
+      <c r="BB83" s="49"/>
+      <c r="BC83" s="49"/>
+    </row>
+    <row r="84" spans="1:55" s="16" customFormat="1" ht="17.25" customHeight="1">
       <c r="A84" s="30"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
       <c r="D84" s="17"/>
       <c r="E84" s="25"/>
     </row>
-    <row r="85" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="85" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A85" s="31"/>
-      <c r="B85" s="42" t="s">
+      <c r="B85" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="C85" s="42"/>
-      <c r="D85" s="42"/>
+      <c r="C85" s="43"/>
+      <c r="D85" s="43"/>
       <c r="E85" s="26"/>
       <c r="G85" s="16"/>
       <c r="H85" s="16"/>
     </row>
-    <row r="86" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="86" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A86" s="32"/>
       <c r="B86" s="13" t="s">
         <v>19</v>
@@ -2285,8 +2545,11 @@
       </c>
       <c r="E86" s="26"/>
       <c r="F86" s="28"/>
-    </row>
-    <row r="87" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+      <c r="G86" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A87" s="33"/>
       <c r="B87" s="8" t="s">
         <v>21</v>
@@ -2295,13 +2558,13 @@
       <c r="D87" s="8"/>
       <c r="E87" s="26"/>
     </row>
-    <row r="88" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="88" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A88" s="33"/>
       <c r="B88" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C88" s="23">
-        <v>260000</v>
+        <v>200000</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="26"/>
@@ -2310,7 +2573,7 @@
       <c r="H88" s="28"/>
       <c r="I88" s="28"/>
     </row>
-    <row r="89" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="89" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A89" s="33"/>
       <c r="B89" s="8" t="s">
         <v>22</v>
@@ -2323,7 +2586,7 @@
       <c r="H89" s="28"/>
       <c r="I89" s="28"/>
     </row>
-    <row r="90" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="90" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A90" s="33"/>
       <c r="B90" s="8" t="s">
         <v>23</v>
@@ -2333,7 +2596,7 @@
       <c r="E90" s="26"/>
       <c r="F90" s="28"/>
     </row>
-    <row r="91" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="91" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A91" s="33"/>
       <c r="B91" s="8" t="s">
         <v>24</v>
@@ -2343,7 +2606,7 @@
       <c r="E91" s="26"/>
       <c r="F91" s="28"/>
     </row>
-    <row r="92" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="92" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A92" s="33"/>
       <c r="B92" s="8" t="s">
         <v>25</v>
@@ -2353,27 +2616,27 @@
       <c r="E92" s="26"/>
       <c r="F92" s="28"/>
     </row>
-    <row r="93" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1">
+    <row r="93" spans="1:55" s="6" customFormat="1" ht="15.75" customHeight="1">
       <c r="A93" s="32"/>
       <c r="B93" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C93" s="24">
         <f>SUBTOTAL(9,C87:C92)</f>
-        <v>260000</v>
+        <v>200000</v>
       </c>
       <c r="D93" s="15"/>
       <c r="E93" s="26"/>
       <c r="F93" s="28"/>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:55">
       <c r="A94" s="34"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="27"/>
       <c r="F94" s="29"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:55">
       <c r="E95" s="27"/>
     </row>
   </sheetData>

</xml_diff>